<commit_message>
Hinzufügen der Heizungsoptimierung bei der BAFA Einzelmaßnahme
</commit_message>
<xml_diff>
--- a/H-D-BnDTool Rechnungsvorlage.xlsx
+++ b/H-D-BnDTool Rechnungsvorlage.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="B:\Vorlagen Berichte\09 Förderunterlagen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14623050-1835-4356-9D4F-93950188C2CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33DFAEDA-3CF3-452F-A0D3-A5DE4007CFF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{12352447-F054-48FD-8709-725D4E514B07}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{12352447-F054-48FD-8709-725D4E514B07}"/>
   </bookViews>
   <sheets>
     <sheet name="KfW" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="29">
   <si>
     <t>Rechnungsaussteller</t>
   </si>
@@ -117,13 +117,13 @@
     <t>Summe Gebäudehülle:</t>
   </si>
   <si>
-    <t>Einzelmaßnahme: 1=Gebäudehülle; 2=Fachplanung; 3=Wärmepumpe; 4=Beleuchtung</t>
-  </si>
-  <si>
     <t>Summe Heizung:</t>
   </si>
   <si>
     <t>Summe Sonstiges:</t>
+  </si>
+  <si>
+    <t>Einzelmaßnahme: 1=Gebäudehülle; 2=Fachplanung; 3=Wärmepumpe; 4=Beleuchtung; 5=Heizungsoptimierung</t>
   </si>
 </sst>
 </file>
@@ -539,9 +539,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32BFC05A-16B3-4E70-BDBD-58DE762D6AF5}">
   <dimension ref="A1:I77"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="A8" sqref="A8:F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -909,7 +909,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BDAE1D7-3F95-4BE3-8289-8F4A018DC930}">
   <dimension ref="A1:I76"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
@@ -947,25 +947,25 @@
         <v>25</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>22</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>8</v>
       </c>
       <c r="F4" s="2">
         <f>SUMIF($A$7:$A$107,"1",$G$7:$G$107)</f>
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="G4" s="2">
         <f>SUMIF($A$7:$A$107,"3",$G$7:$G$107)</f>
@@ -973,7 +973,7 @@
       </c>
       <c r="H4" s="2">
         <f>SUMIF($A$7:$A$107,"2",$G$7:$G$107)</f>
-        <v>2000</v>
+        <v>0</v>
       </c>
       <c r="I4" s="2">
         <f>SUMIF($A$7:$A$107,"4",$G$7:$G$107)</f>
@@ -1025,9 +1025,7 @@
       <c r="F7" s="7">
         <v>1000</v>
       </c>
-      <c r="G7" s="7">
-        <v>1000</v>
-      </c>
+      <c r="G7" s="7"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
@@ -1048,18 +1046,50 @@
       <c r="F8" s="7">
         <v>2000</v>
       </c>
-      <c r="G8" s="7">
-        <v>2000</v>
-      </c>
+      <c r="G8" s="7"/>
       <c r="I8" s="2"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E9" s="1"/>
+      <c r="A9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" s="7">
+        <v>1000</v>
+      </c>
       <c r="G9" s="7"/>
       <c r="I9" s="2"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E10" s="1"/>
+      <c r="A10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" s="7">
+        <v>2000</v>
+      </c>
       <c r="G10" s="7"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>